<commit_message>
[System Variable] - [`nexial.quiet`]: *NEW* System variable to drastically reduce console logging. Default is false.
[aws.sqs commands]
- [`receiveMessage(profile,queue,var)`]: no message received no longer result in a FAIL to the corresponding step.
- [`receiveMessages(profile,queue,var)`]: no message received no longer result in a FAIL to the corresponding step.
- [`purgeQueue(profile,queue,var)`]: **NEW** command to clear out all messages in target SQS queue.

[base commands]
- [`repeatUntil(steps,maxWaitMs)`]: additional logging to indicate the start of each loop.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/execution-meta/artifact/script/execution-meta.xlsx
+++ b/examples/execution-meta/artifact/script/execution-meta.xlsx
@@ -50,7 +50,7 @@
     <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
     <definedName name="xml">'#system'!$AD$2:$AD$21</definedName>
     <definedName name="macro">'#system'!$O$2:$O$4</definedName>
-    <definedName name="aws.sqs">'#system'!$D$2:$D$5</definedName>
+    <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="localdb">'#system'!$N$2:$N$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9295" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9830" uniqueCount="540">
   <si>
     <t>description</t>
   </si>
@@ -1943,13 +1943,16 @@
   <si>
     <t>exportEXCEL(sql,output,sheet,start)</t>
   </si>
+  <si>
+    <t>purgeQueue(profile,queue,var)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="284" x14ac:knownFonts="1">
+  <fonts count="300" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3750,8 +3753,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="490">
+  <fills count="520">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6524,8 +6628,178 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="479">
+  <borders count="507">
     <border>
       <left/>
       <right/>
@@ -11357,6 +11631,288 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -11364,7 +11920,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="309">
+  <cellXfs count="325">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -12261,52 +12817,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="459" fontId="267" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="268" fillId="462" borderId="458" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="458" fillId="462" fontId="268" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="269" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="269" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="270" fillId="465" borderId="462" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="462" fillId="465" fontId="270" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="271" fillId="468" borderId="466" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="466" fillId="468" fontId="271" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="272" fillId="471" borderId="466" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="466" fillId="471" fontId="272" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="273" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="273" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="274" fillId="474" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="474" fontId="274" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="275" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="275" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="276" fillId="477" borderId="470" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="470" fillId="477" fontId="276" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="277" fillId="480" borderId="474" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="474" fillId="480" fontId="277" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="278" fillId="483" borderId="478" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="478" fillId="483" fontId="278" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="279" fillId="483" borderId="478" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="478" fillId="483" fontId="279" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="280" fillId="471" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="471" fontId="280" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="281" fillId="486" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="486" fontId="281" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="282" fillId="471" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="471" fontId="282" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="283" fillId="489" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="489" fontId="283" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="284" fillId="492" borderId="486" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="285" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="286" fillId="495" borderId="490" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="287" fillId="498" borderId="494" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="288" fillId="501" borderId="494" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="289" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="290" fillId="504" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="291" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="292" fillId="507" borderId="498" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="293" fillId="510" borderId="502" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="294" fillId="513" borderId="506" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="295" fillId="513" borderId="506" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="296" fillId="501" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="297" fillId="516" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="298" fillId="501" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="299" fillId="519" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -12837,7 +13441,7 @@
         <v>455</v>
       </c>
       <c r="D3" t="s">
-        <v>501</v>
+        <v>539</v>
       </c>
       <c r="E3" t="s">
         <v>456</v>
@@ -12920,7 +13524,7 @@
         <v>372</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -13003,7 +13607,7 @@
         <v>373</v>
       </c>
       <c r="D5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
         <v>457</v>
@@ -13072,6 +13676,9 @@
       </c>
       <c r="B6" t="s">
         <v>374</v>
+      </c>
+      <c r="D6" t="s">
+        <v>503</v>
       </c>
       <c r="E6" t="s">
         <v>27</v>

</xml_diff>